<commit_message>
Se realiza el CRUD de equipos
</commit_message>
<xml_diff>
--- a/HISTORIAS DE USUARIO EXCEL V2.0.xlsx
+++ b/HISTORIAS DE USUARIO EXCEL V2.0.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SALVAVIDAS\OneDrive - Eficacia\Mis documentos\EFICACIA\DOROZCO\MINTIC2022\C3-PRG\Proyecto\ProyectoTic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C212D0FE-7C1B-4F26-B562-DB9970AD24A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C7A812-4CCE-491B-A8D8-7421562A2C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="806" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="806" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BACKLOG" sheetId="7" r:id="rId1"/>
@@ -2092,22 +2092,22 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2128,22 +2128,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2475,6 +2475,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A2:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2517,10 +2518,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:C28"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B34" sqref="B34:C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2751,10 +2753,10 @@
       <c r="A34" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="23" t="s">
+      <c r="B34" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C34" s="23"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="24" t="s">
@@ -3004,6 +3006,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:I55"/>
   <sheetViews>
     <sheetView topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
@@ -3454,9 +3457,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:I65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="A60" sqref="A60:C61"/>
     </sheetView>
   </sheetViews>
@@ -3903,16 +3907,16 @@
       <c r="C59" s="30"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" s="49" t="s">
+      <c r="A60" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="B60" s="50"/>
-      <c r="C60" s="51"/>
+      <c r="B60" s="38"/>
+      <c r="C60" s="39"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="52"/>
-      <c r="B61" s="53"/>
-      <c r="C61" s="54"/>
+      <c r="A61" s="40"/>
+      <c r="B61" s="41"/>
+      <c r="C61" s="42"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
@@ -3996,10 +4000,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Hoja5"/>
   <dimension ref="A1:C522"/>
   <sheetViews>
-    <sheetView topLeftCell="A509" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D517" sqref="D517"/>
+    <sheetView tabSelected="1" topLeftCell="A161" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A170" sqref="A170:C171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4024,10 +4029,10 @@
       <c r="A2" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C2" s="23"/>
+      <c r="C2" s="25"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
@@ -4046,16 +4051,16 @@
       <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="24"/>
-      <c r="C5" s="24"/>
+      <c r="B5" s="25"/>
+      <c r="C5" s="25"/>
     </row>
     <row r="6" spans="1:3" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24"/>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="25"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="23" t="s">
@@ -4094,10 +4099,10 @@
       <c r="A13" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="25"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
@@ -4116,16 +4121,16 @@
       <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
+      <c r="A16" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
+      <c r="B16" s="25"/>
+      <c r="C16" s="25"/>
     </row>
     <row r="17" spans="1:3" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="24"/>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
+      <c r="A17" s="25"/>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="23" t="s">
@@ -4164,10 +4169,10 @@
       <c r="A24" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="23"/>
+      <c r="C24" s="25"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
@@ -4186,16 +4191,16 @@
       <c r="C26" s="23"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
+      <c r="A27" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="25"/>
+      <c r="C27" s="25"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="24"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
+      <c r="A28" s="25"/>
+      <c r="B28" s="25"/>
+      <c r="C28" s="25"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="23" t="s">
@@ -4234,10 +4239,10 @@
       <c r="A35" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="C35" s="23"/>
+      <c r="C35" s="25"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="24" t="s">
@@ -4256,16 +4261,16 @@
       <c r="C37" s="23"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="24" t="s">
+      <c r="A38" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="B38" s="24"/>
-      <c r="C38" s="24"/>
+      <c r="B38" s="25"/>
+      <c r="C38" s="25"/>
     </row>
     <row r="39" spans="1:3" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="24"/>
-      <c r="B39" s="24"/>
-      <c r="C39" s="24"/>
+      <c r="A39" s="25"/>
+      <c r="B39" s="25"/>
+      <c r="C39" s="25"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
@@ -4304,10 +4309,10 @@
       <c r="A46" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B46" s="23" t="s">
+      <c r="B46" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="C46" s="23"/>
+      <c r="C46" s="25"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="24" t="s">
@@ -4326,16 +4331,16 @@
       <c r="C48" s="23"/>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
+      <c r="A49" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="25"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="24"/>
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
+      <c r="A50" s="25"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="25"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="23" t="s">
@@ -4934,10 +4939,10 @@
       <c r="A145" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B145" s="23" t="s">
+      <c r="B145" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="C145" s="23"/>
+      <c r="C145" s="25"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" s="24" t="s">
@@ -4956,16 +4961,16 @@
       <c r="C147" s="23"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A148" s="24" t="s">
+      <c r="A148" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="B148" s="24"/>
-      <c r="C148" s="24"/>
+      <c r="B148" s="25"/>
+      <c r="C148" s="25"/>
     </row>
     <row r="149" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A149" s="24"/>
-      <c r="B149" s="24"/>
-      <c r="C149" s="24"/>
+      <c r="A149" s="25"/>
+      <c r="B149" s="25"/>
+      <c r="C149" s="25"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" s="23" t="s">
@@ -5074,10 +5079,10 @@
       <c r="A167" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B167" s="23" t="s">
+      <c r="B167" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="C167" s="23"/>
+      <c r="C167" s="25"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" s="24" t="s">
@@ -5364,10 +5369,10 @@
       <c r="A213" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B213" s="23" t="s">
+      <c r="B213" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="C213" s="23"/>
+      <c r="C213" s="25"/>
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" s="24" t="s">
@@ -5386,16 +5391,16 @@
       <c r="C215" s="23"/>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="24" t="s">
+      <c r="A216" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="B216" s="24"/>
-      <c r="C216" s="24"/>
+      <c r="B216" s="25"/>
+      <c r="C216" s="25"/>
     </row>
     <row r="217" spans="1:3" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="24"/>
-      <c r="B217" s="24"/>
-      <c r="C217" s="24"/>
+      <c r="A217" s="25"/>
+      <c r="B217" s="25"/>
+      <c r="C217" s="25"/>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" s="23" t="s">
@@ -7701,6 +7706,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:C132"/>
   <sheetViews>
     <sheetView topLeftCell="A124" workbookViewId="0">
@@ -7816,16 +7822,16 @@
       <c r="C15" s="30"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="37" t="s">
+      <c r="A16" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="B16" s="38"/>
-      <c r="C16" s="39"/>
+      <c r="B16" s="50"/>
+      <c r="C16" s="51"/>
     </row>
     <row r="17" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="40"/>
-      <c r="B17" s="41"/>
-      <c r="C17" s="42"/>
+      <c r="A17" s="52"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="29" t="s">
@@ -7884,16 +7890,16 @@
       <c r="C26" s="30"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="37" t="s">
+      <c r="A27" s="49" t="s">
         <v>85</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="39"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="51"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="40"/>
-      <c r="B28" s="41"/>
-      <c r="C28" s="42"/>
+      <c r="A28" s="52"/>
+      <c r="B28" s="53"/>
+      <c r="C28" s="54"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="29" t="s">
@@ -7952,16 +7958,16 @@
       <c r="C37" s="30"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="37" t="s">
+      <c r="A38" s="49" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="38"/>
-      <c r="C38" s="39"/>
+      <c r="B38" s="50"/>
+      <c r="C38" s="51"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="40"/>
-      <c r="B39" s="41"/>
-      <c r="C39" s="42"/>
+      <c r="A39" s="52"/>
+      <c r="B39" s="53"/>
+      <c r="C39" s="54"/>
     </row>
     <row r="40" spans="1:3" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="29" t="s">
@@ -8020,16 +8026,16 @@
       <c r="C48" s="30"/>
     </row>
     <row r="49" spans="1:3" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="37" t="s">
+      <c r="A49" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="38"/>
-      <c r="C49" s="39"/>
+      <c r="B49" s="50"/>
+      <c r="C49" s="51"/>
     </row>
     <row r="50" spans="1:3" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="40"/>
-      <c r="B50" s="41"/>
-      <c r="C50" s="42"/>
+      <c r="A50" s="52"/>
+      <c r="B50" s="53"/>
+      <c r="C50" s="54"/>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="29" t="s">
@@ -8088,16 +8094,16 @@
       <c r="C59" s="30"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="37" t="s">
+      <c r="A60" s="49" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="38"/>
-      <c r="C60" s="39"/>
+      <c r="B60" s="50"/>
+      <c r="C60" s="51"/>
     </row>
     <row r="61" spans="1:3" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40"/>
-      <c r="B61" s="41"/>
-      <c r="C61" s="42"/>
+      <c r="A61" s="52"/>
+      <c r="B61" s="53"/>
+      <c r="C61" s="54"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="29" t="s">
@@ -8156,16 +8162,16 @@
       <c r="C70" s="30"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="37" t="s">
+      <c r="A71" s="49" t="s">
         <v>88</v>
       </c>
-      <c r="B71" s="38"/>
-      <c r="C71" s="39"/>
+      <c r="B71" s="50"/>
+      <c r="C71" s="51"/>
     </row>
     <row r="72" spans="1:3" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="40"/>
-      <c r="B72" s="41"/>
-      <c r="C72" s="42"/>
+      <c r="A72" s="52"/>
+      <c r="B72" s="53"/>
+      <c r="C72" s="54"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="29" t="s">
@@ -8224,16 +8230,16 @@
       <c r="C82" s="30"/>
     </row>
     <row r="83" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="37" t="s">
+      <c r="A83" s="49" t="s">
         <v>95</v>
       </c>
-      <c r="B83" s="38"/>
-      <c r="C83" s="39"/>
+      <c r="B83" s="50"/>
+      <c r="C83" s="51"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="40"/>
-      <c r="B84" s="41"/>
-      <c r="C84" s="42"/>
+      <c r="A84" s="52"/>
+      <c r="B84" s="53"/>
+      <c r="C84" s="54"/>
     </row>
     <row r="85" spans="1:3" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="29" t="s">
@@ -8292,16 +8298,16 @@
       <c r="C93" s="30"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="37" t="s">
+      <c r="A94" s="49" t="s">
         <v>76</v>
       </c>
-      <c r="B94" s="38"/>
-      <c r="C94" s="39"/>
+      <c r="B94" s="50"/>
+      <c r="C94" s="51"/>
     </row>
     <row r="95" spans="1:3" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A95" s="40"/>
-      <c r="B95" s="41"/>
-      <c r="C95" s="42"/>
+      <c r="A95" s="52"/>
+      <c r="B95" s="53"/>
+      <c r="C95" s="54"/>
     </row>
     <row r="96" spans="1:3" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96" s="29" t="s">
@@ -8360,16 +8366,16 @@
       <c r="C104" s="30"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="37" t="s">
+      <c r="A105" s="49" t="s">
         <v>78</v>
       </c>
-      <c r="B105" s="38"/>
-      <c r="C105" s="39"/>
+      <c r="B105" s="50"/>
+      <c r="C105" s="51"/>
     </row>
     <row r="106" spans="1:3" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="40"/>
-      <c r="B106" s="41"/>
-      <c r="C106" s="42"/>
+      <c r="A106" s="52"/>
+      <c r="B106" s="53"/>
+      <c r="C106" s="54"/>
     </row>
     <row r="107" spans="1:3" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="29" t="s">
@@ -8428,16 +8434,16 @@
       <c r="C115" s="30"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="37" t="s">
+      <c r="A116" s="49" t="s">
         <v>90</v>
       </c>
-      <c r="B116" s="38"/>
-      <c r="C116" s="39"/>
+      <c r="B116" s="50"/>
+      <c r="C116" s="51"/>
     </row>
     <row r="117" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A117" s="40"/>
-      <c r="B117" s="41"/>
-      <c r="C117" s="42"/>
+      <c r="A117" s="52"/>
+      <c r="B117" s="53"/>
+      <c r="C117" s="54"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="29" t="s">
@@ -8496,16 +8502,16 @@
       <c r="C126" s="30"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="37" t="s">
+      <c r="A127" s="49" t="s">
         <v>92</v>
       </c>
-      <c r="B127" s="38"/>
-      <c r="C127" s="39"/>
+      <c r="B127" s="50"/>
+      <c r="C127" s="51"/>
     </row>
     <row r="128" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A128" s="40"/>
-      <c r="B128" s="41"/>
-      <c r="C128" s="42"/>
+      <c r="A128" s="52"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="54"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="29" t="s">
@@ -8547,6 +8553,7 @@
     <mergeCell ref="A92:B92"/>
     <mergeCell ref="A87:C87"/>
     <mergeCell ref="A88:C88"/>
+    <mergeCell ref="B113:C113"/>
     <mergeCell ref="A114:B114"/>
     <mergeCell ref="B91:C91"/>
     <mergeCell ref="A115:C115"/>
@@ -8554,21 +8561,25 @@
     <mergeCell ref="A93:C93"/>
     <mergeCell ref="A94:C95"/>
     <mergeCell ref="A96:C96"/>
+    <mergeCell ref="A63:C63"/>
     <mergeCell ref="A85:C85"/>
     <mergeCell ref="A86:C86"/>
     <mergeCell ref="A109:C109"/>
     <mergeCell ref="A110:C110"/>
-    <mergeCell ref="B113:C113"/>
-    <mergeCell ref="A48:C48"/>
     <mergeCell ref="B80:C80"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A82:C82"/>
     <mergeCell ref="A83:C84"/>
-    <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A43:C43"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="B68:C68"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A71:C72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:C74"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A76:C76"/>
     <mergeCell ref="A132:C132"/>
     <mergeCell ref="A118:C118"/>
     <mergeCell ref="A119:C119"/>
@@ -8581,32 +8592,27 @@
     <mergeCell ref="A131:C131"/>
     <mergeCell ref="A125:B125"/>
     <mergeCell ref="B124:C124"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A71:C72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:C74"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A76:C76"/>
-    <mergeCell ref="A63:C63"/>
     <mergeCell ref="A29:C29"/>
     <mergeCell ref="A30:C30"/>
     <mergeCell ref="A31:C31"/>
     <mergeCell ref="A32:C32"/>
     <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A38:C39"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A43:C43"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A48:C48"/>
     <mergeCell ref="A58:B58"/>
     <mergeCell ref="A59:C59"/>
     <mergeCell ref="A60:C61"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A52:C52"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A38:C39"/>
-    <mergeCell ref="A40:C40"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A27:C28"/>
     <mergeCell ref="A20:C20"/>

</xml_diff>